<commit_message>
(GridData->simple) Version 2.0 of DC Power Flow
</commit_message>
<xml_diff>
--- a/tests/dummy_data/dc_power_flow/ConfigFiles/Config_BOLIVIA_POWERFLOWDC_TEST.xlsx
+++ b/tests/dummy_data/dc_power_flow/ConfigFiles/Config_BOLIVIA_POWERFLOWDC_TEST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navia\Desktop\EJEMPLO\BaseDatos_DispaSET\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navia\Dispa-SET\tests\dummy_data\dc_power_flow\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077381B7-B384-4C9B-9F16-039033AC8FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEEAC9D-6DDA-49A9-81F2-893E7D1ABC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -638,58 +638,58 @@
     <t>Boundary Sector Reservoir Level</t>
   </si>
   <si>
+    <t>Transmision grid type</t>
+  </si>
+  <si>
+    <t>DC-Power Flow</t>
+  </si>
+  <si>
+    <t>Transmission grid type</t>
+  </si>
+  <si>
+    <t>NTC/DC-Power Flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These parameters influence how transmission lines are modeled </t>
+  </si>
+  <si>
+    <t>Demand/Demand_AREAS.csv</t>
+  </si>
+  <si>
+    <t>RenewablesAF/RenewablesAF.csv</t>
+  </si>
+  <si>
+    <t>ScaledInflows/1984.csv</t>
+  </si>
+  <si>
+    <t>GeoCoordinates_AREAS.csv</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>Dispa-SET Configuration File (v20.04)</t>
+  </si>
+  <si>
+    <t>Grid Data</t>
+  </si>
+  <si>
+    <t>GridData/GridData.csv</t>
+  </si>
+  <si>
     <t>Simulations/BOLIVIA_POWERFLOWDC_TEST</t>
   </si>
   <si>
-    <t>Transmision grid type</t>
-  </si>
-  <si>
-    <t>DC-Power Flow</t>
-  </si>
-  <si>
-    <t>Transmission grid type</t>
-  </si>
-  <si>
-    <t>NTC/DC-Power Flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These parameters influence how transmission lines are modeled </t>
-  </si>
-  <si>
-    <t>Demand/Demand_AREAS.csv</t>
+    <t>NTC/NTC.csv</t>
   </si>
   <si>
     <t>PowerPlantData/PowerPlantData_AREAS.csv</t>
-  </si>
-  <si>
-    <t>RenewablesAF/RenewablesAF.csv</t>
-  </si>
-  <si>
-    <t>NTC/NTC_DCPF1.csv</t>
-  </si>
-  <si>
-    <t>ScaledInflows/1984.csv</t>
-  </si>
-  <si>
-    <t>GeoCoordinates_AREAS.csv</t>
-  </si>
-  <si>
-    <t>PTDF/PTDF.csv</t>
-  </si>
-  <si>
-    <t>PTDF Matrix</t>
-  </si>
-  <si>
-    <t>CE</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>SU</t>
-  </si>
-  <si>
-    <t>Dispa-SET Configuration File (v20.04)</t>
   </si>
 </sst>
 </file>
@@ -1476,8 +1476,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1495,7 +1495,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -1688,7 +1688,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1752,7 +1752,7 @@
         <v>194</v>
       </c>
       <c r="C39" s="40">
-        <v>5.9999999999999995E-4</v>
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1829,7 +1829,7 @@
         <v>20</v>
       </c>
       <c r="C59" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>60</v>
@@ -1939,16 +1939,16 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B80" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="B80" s="27" t="s">
+      <c r="C80" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="H80" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2090,7 +2090,7 @@
         <v>9</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>61</v>
@@ -2139,7 +2139,7 @@
         <v>9</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>61</v>
@@ -2156,7 +2156,7 @@
         <v>9</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>61</v>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="F130" s="5">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="H130" s="11" t="s">
         <v>43</v>
@@ -2191,7 +2191,7 @@
         <v>9</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>61</v>
@@ -2223,7 +2223,7 @@
         <v>9</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D133" s="18" t="s">
         <v>61</v>
@@ -2277,7 +2277,7 @@
         <v>9</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>61</v>
@@ -2363,7 +2363,7 @@
         <v>9</v>
       </c>
       <c r="C146" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D146" s="18" t="s">
         <v>61</v>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="F206" s="5">
-        <v>1501</v>
+        <v>10</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>117</v>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>400</v>
+        <v>1501</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>118</v>
@@ -2822,7 +2822,7 @@
         <v>24</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C226" s="4" t="b">
         <v>1</v>
@@ -2839,7 +2839,7 @@
         <v>25</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>1</v>
@@ -2869,7 +2869,7 @@
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="42"/>
       <c r="B229" s="6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C229" s="4" t="b">
         <v>1</v>
@@ -3710,7 +3710,7 @@
         <v>119</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -3756,7 +3756,7 @@
         <v>120</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>